<commit_message>
Se agrego el proyecto a Github
</commit_message>
<xml_diff>
--- a/uploads/NOTAS 1 Y 2 CORTE.xlsx
+++ b/uploads/NOTAS 1 Y 2 CORTE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DE54F77-CDFF-41D6-B837-D3E82313E811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B894C0-6D17-4535-B93F-E68465A37F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3E59EF60-73BD-4C91-9ADF-EDC4AEBFF000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="24">
   <si>
     <t>PROGRAMA_ACADEMICO</t>
   </si>
@@ -65,28 +65,49 @@
     <t>CONTADURÍA PÚBLICA</t>
   </si>
   <si>
-    <t>ALVAREZ VILLALOBOS DANA VALERIA</t>
-  </si>
-  <si>
     <t>Matriculado</t>
   </si>
   <si>
-    <t>ARGUELLO ROMÁN MARGARETH</t>
-  </si>
-  <si>
-    <t>ARIAS RAMIREZ ANDREA LILIAM</t>
-  </si>
-  <si>
-    <t>AVILA SIERRA CATALINA</t>
-  </si>
-  <si>
-    <t>BARRERA NUÑEZ JUAN PABLO</t>
-  </si>
-  <si>
-    <t>BELTRAN HERNANDEZ LORENA</t>
-  </si>
-  <si>
     <t>BIOETICA</t>
+  </si>
+  <si>
+    <t>Albert Dayhan Diaz</t>
+  </si>
+  <si>
+    <t>Duvan Gutierrez Lobo</t>
+  </si>
+  <si>
+    <t>Daniela Guzman Perez</t>
+  </si>
+  <si>
+    <t>Perez Carmen Andrea</t>
+  </si>
+  <si>
+    <t>Angulo Juan Camilo</t>
+  </si>
+  <si>
+    <t>Cristian Olivar Isaza</t>
+  </si>
+  <si>
+    <t>Thania Milena Perez</t>
+  </si>
+  <si>
+    <t>Marlene Ballena Guzman</t>
+  </si>
+  <si>
+    <t>Jose Sierra Guzman</t>
+  </si>
+  <si>
+    <t>Diego Silva Benavides</t>
+  </si>
+  <si>
+    <t>Camilo Andres Daza</t>
+  </si>
+  <si>
+    <t>Jose Castellano Endry</t>
+  </si>
+  <si>
+    <t>Elvis Galvis Galvis</t>
   </si>
 </sst>
 </file>
@@ -149,7 +170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -158,6 +179,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,11 +517,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C63E89-62F6-40AF-A7BC-82F5B3DEE024}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="48.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -532,45 +557,45 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G2" s="3">
-        <v>4.4000000000000004</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>4.5</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G3" s="3">
         <v>4.2</v>
@@ -583,14 +608,14 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>4.5</v>
@@ -610,25 +635,25 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>4.2</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G5" s="3">
         <v>3.7</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -636,13 +661,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6">
         <v>4.8</v>
@@ -662,13 +687,13 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <v>3.5</v>
@@ -688,13 +713,13 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8">
         <v>4.9000000000000004</v>
@@ -714,13 +739,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9">
         <v>4.3</v>
@@ -740,13 +765,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10">
         <v>3.9</v>
@@ -766,13 +791,13 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11">
         <v>4.8</v>
@@ -792,13 +817,13 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12">
         <v>4.2</v>
@@ -818,13 +843,13 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -844,13 +869,13 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14">
         <v>4.0999999999999996</v>
@@ -869,14 +894,14 @@
       <c r="A15" t="s">
         <v>8</v>
       </c>
-      <c r="B15" t="s">
-        <v>12</v>
+      <c r="B15" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15">
         <v>4.5999999999999996</v>
@@ -895,14 +920,14 @@
       <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B16" t="s">
-        <v>13</v>
+      <c r="B16" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16">
         <v>4.4000000000000004</v>
@@ -925,10 +950,10 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E17">
         <v>4.4000000000000004</v>
@@ -948,13 +973,13 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18">
         <v>3.6</v>
@@ -974,13 +999,13 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19">
         <v>4.2</v>
@@ -1000,13 +1025,13 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20">
         <v>4.7</v>
@@ -1026,13 +1051,13 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E21">
         <v>5</v>
@@ -1052,13 +1077,13 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E22">
         <v>3.5</v>
@@ -1078,13 +1103,13 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E23">
         <v>4.7</v>
@@ -1104,13 +1129,13 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E24">
         <v>3.2</v>
@@ -1130,13 +1155,13 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E25">
         <v>4.5</v>
@@ -1156,13 +1181,13 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E26">
         <v>4.7</v>
@@ -1181,14 +1206,14 @@
       <c r="A27" t="s">
         <v>8</v>
       </c>
-      <c r="B27" t="s">
-        <v>14</v>
+      <c r="B27" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E27">
         <v>4.5</v>
@@ -1207,14 +1232,14 @@
       <c r="A28" t="s">
         <v>8</v>
       </c>
-      <c r="B28" t="s">
-        <v>15</v>
+      <c r="B28" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E28">
         <v>4.4000000000000004</v>
@@ -1234,13 +1259,13 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E29">
         <v>5</v>
@@ -1260,13 +1285,13 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E30">
         <v>4.7</v>

</xml_diff>